<commit_message>
Got vsc derivatives and 6 bus system working fine
</commit_message>
<xml_diff>
--- a/src/tests/output/tuc_17_1_ieee14_cim_converter.xlsx
+++ b/src/tests/output/tuc_17_1_ieee14_cim_converter.xlsx
@@ -478,7 +478,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>21:59:12</t>
+          <t>00:49:20</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -516,7 +516,7 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>21:59:12</t>
+          <t>00:49:20</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -554,7 +554,7 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>21:59:12</t>
+          <t>00:49:20</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -592,7 +592,7 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>21:59:12</t>
+          <t>00:49:20</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -630,7 +630,7 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>21:59:12</t>
+          <t>00:49:20</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>21:59:12</t>
+          <t>00:49:20</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -706,7 +706,7 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>21:59:12</t>
+          <t>00:49:20</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -744,7 +744,7 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>21:59:12</t>
+          <t>00:49:20</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -782,7 +782,7 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>21:59:12</t>
+          <t>00:49:20</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -820,7 +820,7 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>21:59:12</t>
+          <t>00:49:20</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -858,7 +858,7 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>21:59:12</t>
+          <t>00:49:20</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -896,7 +896,7 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>21:59:12</t>
+          <t>00:49:20</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -934,7 +934,7 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>21:59:12</t>
+          <t>00:49:20</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -972,7 +972,7 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>21:59:12</t>
+          <t>00:49:20</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">

</xml_diff>